<commit_message>
changes to this if it matters
</commit_message>
<xml_diff>
--- a/ExperimentalResults.xlsx
+++ b/ExperimentalResults.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/local/QUAKER/gvanaken/Desktop/registrar-problem/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gavan\OneDrive\Documents\Senior Year\Analysis of Algorithms\registrar-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5304BC7-AD19-5D42-9C30-2E2A6648CA3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E2572FED-BCA5-408A-AB4D-6280084B890F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" xr2:uid="{8DD08929-D612-4643-BC99-4480884B8417}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40965" windowHeight="23040" xr2:uid="{8DD08929-D612-4643-BC99-4480884B8417}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -68,9 +68,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,8 +107,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -160,14 +160,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Running</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t> Time as a Function of Number of Classes</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -493,9 +493,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Log(Sqrt(t))</a:t>
+                  <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Log(n)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -596,13 +601,27 @@
               <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      </a:sysClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -610,9 +629,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Log(n)</a:t>
+                  <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Log(Sqrt(t))</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -628,13 +652,27 @@
             <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
+                    <a:sysClr val="windowText" lastClr="000000">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    </a:sysClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1634,17 +1672,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9284535-B132-3346-988B-22D725AB39E3}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="11" max="11" width="19.1640625" customWidth="1"/>
+    <col min="11" max="11" width="19.125" customWidth="1"/>
     <col min="12" max="12" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1682,7 +1720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1708,23 +1746,23 @@
         <v>637</v>
       </c>
       <c r="I2">
-        <f>H2/G2</f>
+        <f t="shared" ref="I2:I8" si="0">H2/G2</f>
         <v>0.79625000000000001</v>
       </c>
       <c r="J2">
-        <f>SQRT(F2)</f>
+        <f t="shared" ref="J2:J8" si="1">SQRT(F2)</f>
         <v>0.11290283137149396</v>
       </c>
       <c r="K2">
-        <f>LOG(B2)</f>
+        <f t="shared" ref="K2:K8" si="2">LOG(B2)</f>
         <v>1.3010299956639813</v>
       </c>
       <c r="L2">
-        <f>LOG(J2)</f>
+        <f t="shared" ref="L2:L8" si="3">LOG(J2)</f>
         <v>-0.94729516672341674</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1750,23 +1788,23 @@
         <v>324</v>
       </c>
       <c r="I3">
-        <f>H3/G3</f>
+        <f t="shared" si="0"/>
         <v>0.81</v>
       </c>
       <c r="J3">
-        <f>SQRT(F3)</f>
+        <f t="shared" si="1"/>
         <v>9.714956444735097E-2</v>
       </c>
       <c r="K3">
-        <f>LOG(B3)</f>
+        <f t="shared" si="2"/>
         <v>1.3010299956639813</v>
       </c>
       <c r="L3">
-        <f>LOG(J3)</f>
+        <f t="shared" si="3"/>
         <v>-1.0125591421412556</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>7</v>
       </c>
@@ -1792,23 +1830,23 @@
         <v>1469</v>
       </c>
       <c r="I4">
-        <f>H4/G4</f>
+        <f t="shared" si="0"/>
         <v>0.91812499999999997</v>
       </c>
       <c r="J4">
-        <f>SQRT(F4)</f>
+        <f t="shared" si="1"/>
         <v>0.19749935391489259</v>
       </c>
       <c r="K4">
-        <f>LOG(B4)</f>
+        <f t="shared" si="2"/>
         <v>1.6020599913279623</v>
       </c>
       <c r="L4">
-        <f>LOG(J4)</f>
+        <f t="shared" si="3"/>
         <v>-0.7044343207547662</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>18</v>
       </c>
@@ -1834,23 +1872,23 @@
         <v>3714</v>
       </c>
       <c r="I5">
-        <f>H5/G5</f>
+        <f t="shared" si="0"/>
         <v>0.92849999999999999</v>
       </c>
       <c r="J5">
-        <f>SQRT(F5)</f>
+        <f t="shared" si="1"/>
         <v>2.2752591205618757</v>
       </c>
       <c r="K5">
-        <f>LOG(B5)</f>
+        <f t="shared" si="2"/>
         <v>2.6989700043360187</v>
       </c>
       <c r="L5">
-        <f>LOG(J5)</f>
+        <f t="shared" si="3"/>
         <v>0.35703086394779393</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1876,23 +1914,23 @@
         <v>749</v>
       </c>
       <c r="I6">
-        <f>H6/G6</f>
+        <f t="shared" si="0"/>
         <v>0.93625000000000003</v>
       </c>
       <c r="J6">
-        <f>SQRT(F6)</f>
+        <f t="shared" si="1"/>
         <v>0.18668953255980905</v>
       </c>
       <c r="K6">
-        <f>LOG(B6)</f>
+        <f t="shared" si="2"/>
         <v>1.6020599913279623</v>
       </c>
       <c r="L6">
-        <f>LOG(J6)</f>
+        <f t="shared" si="3"/>
         <v>-0.72888003169717241</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>15</v>
       </c>
@@ -1918,23 +1956,23 @@
         <v>3752</v>
       </c>
       <c r="I7">
-        <f>H7/G7</f>
+        <f t="shared" si="0"/>
         <v>0.93799999999999994</v>
       </c>
       <c r="J7">
-        <f>SQRT(F7)</f>
+        <f t="shared" si="1"/>
         <v>0.82554642470184558</v>
       </c>
       <c r="K7">
-        <f>LOG(B7)</f>
+        <f t="shared" si="2"/>
         <v>2.3010299956639813</v>
       </c>
       <c r="L7">
-        <f>LOG(J7)</f>
+        <f t="shared" si="3"/>
         <v>-8.3258499112369988E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>19</v>
       </c>
@@ -1960,29 +1998,29 @@
         <v>7536</v>
       </c>
       <c r="I8">
-        <f>H8/G8</f>
+        <f t="shared" si="0"/>
         <v>0.94199999999999995</v>
       </c>
       <c r="J8">
-        <f>SQRT(F8)</f>
+        <f t="shared" si="1"/>
         <v>2.2712604809246342</v>
       </c>
       <c r="K8">
-        <f>LOG(B8)</f>
+        <f t="shared" si="2"/>
         <v>2.6989700043360187</v>
       </c>
       <c r="L8">
-        <f>LOG(J8)</f>
+        <f t="shared" si="3"/>
         <v>0.35626694440953333</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="I9">
         <f>AVERAGE(I1:I8)</f>
         <v>0.89558928571428564</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2008,23 +2046,23 @@
         <v>758</v>
       </c>
       <c r="I10">
-        <f>H10/G10</f>
+        <f t="shared" ref="I10:I24" si="4">H10/G10</f>
         <v>0.94750000000000001</v>
       </c>
       <c r="J10">
-        <f>SQRT(F10)</f>
+        <f t="shared" ref="J10:J24" si="5">SQRT(F10)</f>
         <v>0.10547553146583334</v>
       </c>
       <c r="K10">
-        <f>LOG(B10)</f>
+        <f t="shared" ref="K10:K24" si="6">LOG(B10)</f>
         <v>1.3010299956639813</v>
       </c>
       <c r="L10">
-        <f>LOG(J10)</f>
+        <f t="shared" ref="L10:L24" si="7">LOG(J10)</f>
         <v>-0.97684827763513349</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2050,23 +2088,23 @@
         <v>1522</v>
       </c>
       <c r="I11">
-        <f>H11/G11</f>
+        <f t="shared" si="4"/>
         <v>0.95125000000000004</v>
       </c>
       <c r="J11">
-        <f>SQRT(F11)</f>
+        <f t="shared" si="5"/>
         <v>0.30074557798810608</v>
       </c>
       <c r="K11">
-        <f>LOG(B11)</f>
+        <f t="shared" si="6"/>
         <v>1.9030899869919435</v>
       </c>
       <c r="L11">
-        <f>LOG(J11)</f>
+        <f t="shared" si="7"/>
         <v>-0.52180074958905887</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2092,23 +2130,23 @@
         <v>381</v>
       </c>
       <c r="I12">
-        <f>H12/G12</f>
+        <f t="shared" si="4"/>
         <v>0.95250000000000001</v>
       </c>
       <c r="J12">
-        <f>SQRT(F12)</f>
+        <f t="shared" si="5"/>
         <v>7.7479941941124356E-2</v>
       </c>
       <c r="K12">
-        <f>LOG(B12)</f>
+        <f t="shared" si="6"/>
         <v>1.3010299956639813</v>
       </c>
       <c r="L12">
-        <f>LOG(J12)</f>
+        <f t="shared" si="7"/>
         <v>-1.1108107133873455</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2134,23 +2172,23 @@
         <v>2286</v>
       </c>
       <c r="I13">
-        <f>H13/G13</f>
+        <f t="shared" si="4"/>
         <v>0.95250000000000001</v>
       </c>
       <c r="J13">
-        <f>SQRT(F13)</f>
+        <f t="shared" si="5"/>
         <v>0.39586482006488022</v>
       </c>
       <c r="K13">
-        <f>LOG(B13)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L13">
-        <f>LOG(J13)</f>
+        <f t="shared" si="7"/>
         <v>-0.40245309165664384</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>16</v>
       </c>
@@ -2176,23 +2214,23 @@
         <v>7679</v>
       </c>
       <c r="I14">
-        <f>H14/G14</f>
+        <f t="shared" si="4"/>
         <v>0.95987500000000003</v>
       </c>
       <c r="J14">
-        <f>SQRT(F14)</f>
+        <f t="shared" si="5"/>
         <v>0.83719063354232537</v>
       </c>
       <c r="K14">
-        <f>LOG(B14)</f>
+        <f t="shared" si="6"/>
         <v>2.3010299956639813</v>
       </c>
       <c r="L14">
-        <f>LOG(J14)</f>
+        <f t="shared" si="7"/>
         <v>-7.7175639176683894E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2218,23 +2256,23 @@
         <v>3073</v>
       </c>
       <c r="I15">
-        <f>H15/G15</f>
+        <f t="shared" si="4"/>
         <v>0.96031250000000001</v>
       </c>
       <c r="J15">
-        <f>SQRT(F15)</f>
+        <f t="shared" si="5"/>
         <v>0.39934182854667249</v>
       </c>
       <c r="K15">
-        <f>LOG(B15)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L15">
-        <f>LOG(J15)</f>
+        <f t="shared" si="7"/>
         <v>-0.39865519780568653</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>20</v>
       </c>
@@ -2260,23 +2298,23 @@
         <v>19257</v>
       </c>
       <c r="I16">
-        <f>H16/G16</f>
+        <f t="shared" si="4"/>
         <v>0.96284999999999998</v>
       </c>
       <c r="J16">
-        <f>SQRT(F16)</f>
+        <f t="shared" si="5"/>
         <v>2.2670968372149436</v>
       </c>
       <c r="K16">
-        <f>LOG(B16)</f>
+        <f t="shared" si="6"/>
         <v>2.6989700043360187</v>
       </c>
       <c r="L16">
-        <f>LOG(J16)</f>
+        <f t="shared" si="7"/>
         <v>0.35547007106162493</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>10</v>
       </c>
@@ -2302,23 +2340,23 @@
         <v>2312</v>
       </c>
       <c r="I17">
-        <f>H17/G17</f>
+        <f t="shared" si="4"/>
         <v>0.96333333333333337</v>
       </c>
       <c r="J17">
-        <f>SQRT(F17)</f>
+        <f t="shared" si="5"/>
         <v>0.31868647522133725</v>
       </c>
       <c r="K17">
-        <f>LOG(B17)</f>
+        <f t="shared" si="6"/>
         <v>1.9030899869919435</v>
       </c>
       <c r="L17">
-        <f>LOG(J17)</f>
+        <f t="shared" si="7"/>
         <v>-0.49663636721775961</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>6</v>
       </c>
@@ -2344,23 +2382,23 @@
         <v>772</v>
       </c>
       <c r="I18">
-        <f>H18/G18</f>
+        <f t="shared" si="4"/>
         <v>0.96499999999999997</v>
       </c>
       <c r="J18">
-        <f>SQRT(F18)</f>
+        <f t="shared" si="5"/>
         <v>0.14825347736764896</v>
       </c>
       <c r="K18">
-        <f>LOG(B18)</f>
+        <f t="shared" si="6"/>
         <v>1.6020599913279623</v>
       </c>
       <c r="L18">
-        <f>LOG(J18)</f>
+        <f t="shared" si="7"/>
         <v>-0.82899511122595915</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>13</v>
       </c>
@@ -2386,23 +2424,23 @@
         <v>3863</v>
       </c>
       <c r="I19">
-        <f>H19/G19</f>
+        <f t="shared" si="4"/>
         <v>0.96575</v>
       </c>
       <c r="J19">
-        <f>SQRT(F19)</f>
+        <f t="shared" si="5"/>
         <v>0.40466409858548114</v>
       </c>
       <c r="K19">
-        <f>LOG(B19)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L19">
-        <f>LOG(J19)</f>
+        <f t="shared" si="7"/>
         <v>-0.39290532409334028</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>8</v>
       </c>
@@ -2428,23 +2466,23 @@
         <v>1560</v>
       </c>
       <c r="I20">
-        <f>H20/G20</f>
+        <f t="shared" si="4"/>
         <v>0.97499999999999998</v>
       </c>
       <c r="J20">
-        <f>SQRT(F20)</f>
+        <f t="shared" si="5"/>
         <v>0.16610894665670481</v>
       </c>
       <c r="K20">
-        <f>LOG(B20)</f>
+        <f t="shared" si="6"/>
         <v>1.6020599913279623</v>
       </c>
       <c r="L20">
-        <f>LOG(J20)</f>
+        <f t="shared" si="7"/>
         <v>-0.77960697574246407</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>17</v>
       </c>
@@ -2470,23 +2508,23 @@
         <v>11701</v>
       </c>
       <c r="I21">
-        <f>H21/G21</f>
+        <f t="shared" si="4"/>
         <v>0.9750833333333333</v>
       </c>
       <c r="J21">
-        <f>SQRT(F21)</f>
+        <f t="shared" si="5"/>
         <v>0.85531224600259292</v>
       </c>
       <c r="K21">
-        <f>LOG(B21)</f>
+        <f t="shared" si="6"/>
         <v>2.3010299956639813</v>
       </c>
       <c r="L21">
-        <f>LOG(J21)</f>
+        <f t="shared" si="7"/>
         <v>-6.7875309879823917E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>22</v>
       </c>
@@ -2512,23 +2550,23 @@
         <v>156211</v>
       </c>
       <c r="I22">
-        <f>H22/G22</f>
+        <f t="shared" si="4"/>
         <v>0.97631875000000001</v>
       </c>
       <c r="J22">
-        <f>SQRT(F22)</f>
+        <f t="shared" si="5"/>
         <v>10.818842091832193</v>
       </c>
       <c r="K22">
-        <f>LOG(B22)</f>
+        <f t="shared" si="6"/>
         <v>3.3010299956639813</v>
       </c>
       <c r="L22">
-        <f>LOG(J22)</f>
+        <f t="shared" si="7"/>
         <v>1.0341807820240285</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2554,23 +2592,23 @@
         <v>39061</v>
       </c>
       <c r="I23">
-        <f>H23/G23</f>
+        <f t="shared" si="4"/>
         <v>0.97652499999999998</v>
       </c>
       <c r="J23">
-        <f>SQRT(F23)</f>
+        <f t="shared" si="5"/>
         <v>2.3016448545507622</v>
       </c>
       <c r="K23">
-        <f>LOG(B23)</f>
+        <f t="shared" si="6"/>
         <v>2.6989700043360187</v>
       </c>
       <c r="L23">
-        <f>LOG(J23)</f>
+        <f t="shared" si="7"/>
         <v>0.36203831251368634</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>14</v>
       </c>
@@ -2596,19 +2634,19 @@
         <v>7843</v>
       </c>
       <c r="I24">
-        <f>H24/G24</f>
+        <f t="shared" si="4"/>
         <v>0.980375</v>
       </c>
       <c r="J24">
-        <f>SQRT(F24)</f>
+        <f t="shared" si="5"/>
         <v>0.43236443087168952</v>
       </c>
       <c r="K24">
-        <f>LOG(B24)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L24">
-        <f>LOG(J24)</f>
+        <f t="shared" si="7"/>
         <v>-0.36415004115614441</v>
       </c>
     </row>

</xml_diff>